<commit_message>
Working on the Alt versions
</commit_message>
<xml_diff>
--- a/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
+++ b/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF0E22-16EC-444C-BD86-A301C8F138A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F44517-DC74-4FE1-B535-12779914F9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
   <si>
     <t>Message</t>
   </si>
@@ -123,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +146,14 @@
       <color theme="1"/>
       <name val="Aptos Mono"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -176,19 +185,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,6 +694,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="1160" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1CC9AFD0-1337-43EA-AAEE-FAB4629AAF96}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
@@ -1332,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BD705D-A3A8-4C82-9804-A350C1229BB5}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1396,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1502,7 +1541,156 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1" xr:uid="{003280AC-CC62-4129-A983-9A784678E40A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6984DD-D8E9-4573-95DB-78BA80017482}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>20230523</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>19991231</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>20211118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>20001010</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>19910828</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>20090708</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="str" cm="1">
+        <f t="array" ref="A14:A19">_xlfn.MAP(
+    A2:A7,
+    B2:B7,
+    _xlfn.LAMBDA(_xlpm.a,_xlpm.k,
+        _xlfn.LET(
+            _xlpm.s, _xlfn.SEQUENCE(LEN(_xlpm.a)),
+            _xlpm.c, CODE(MID(_xlpm.a, _xlpm.s, 1)),
+            _xlpm.f, FLOOR(_xlpm.c, 32),
+            _xlfn.CONCAT(CHAR(MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26) + _xlpm.f))
+        )
+    )
+)</f>
+        <v>enemy</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <v>battlewon</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <v>bringelephants</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <v>moveforwardarchers</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <v>horsesandcannons</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <v>hailthekingandqueen</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Interim work on alt
</commit_message>
<xml_diff>
--- a/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
+++ b/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F44517-DC74-4FE1-B535-12779914F9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80214398-0B9F-4EA8-A62E-C63E0D8FD910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>Message</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Model Version</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6984DD-D8E9-4573-95DB-78BA80017482}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,36 +1667,277 @@
             _xlpm.s, _xlfn.SEQUENCE(LEN(_xlpm.a)),
             _xlpm.c, CODE(MID(_xlpm.a, _xlpm.s, 1)),
             _xlpm.f, FLOOR(_xlpm.c, 32),
-            _xlfn.CONCAT(CHAR(MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26) + _xlpm.f))
+            _xlfn.CONCAT(CHAR(MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26) + _xlpm.f),_xlpm.f,MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26))
         )
     )
 )</f>
-        <v>enemy</v>
+        <v>enemy969696969651451325</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <v>battlewon</v>
+        <v>battlewon969696969696969696212020125231514</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <v>bringelephants</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>bringelephants9696969696969696969696969696218914751251681142019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <v>moveforwardarchers</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>moveforwardarchers9696969696969696969696969696969696961315225615182311841183851819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <v>horsesandcannons</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>horsesandcannons9696969696969696969696969696969681518195191144311414151419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <v>hailthekingandqueen</v>
+        <v>hailthekingandqueen96969696969696969696969696969696969696819122085119147114417215514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="str" cm="1">
+        <f t="array" ref="B24:B32">MID(A3,_xlfn.SEQUENCE(LEN(A3)),1)</f>
+        <v>c</v>
+      </c>
+      <c r="C24" t="str" cm="1">
+        <f t="array" ref="C24:C32">MID(REPT(B3, 9), _xlfn.SEQUENCE(LEN(A3)), 1)</f>
+        <v>1</v>
+      </c>
+      <c r="D24" cm="1">
+        <f t="array" ref="D24:D32">CODE(_xlfn.ANCHORARRAY(B24))</f>
+        <v>99</v>
+      </c>
+      <c r="E24" cm="1">
+        <f t="array" ref="E24:E32">CODE(_xlfn.ANCHORARRAY(C24))</f>
+        <v>49</v>
+      </c>
+      <c r="F24" cm="1">
+        <f t="array" ref="F24:F32">FLOOR(_xlfn.ANCHORARRAY(D24),32)</f>
+        <v>96</v>
+      </c>
+      <c r="G24">
+        <f>MOD(D24-E24-F24,26)+F24</f>
+        <v>102</v>
+      </c>
+      <c r="H24" t="str">
+        <f>CHAR(G24)</f>
+        <v>f</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <v>j</v>
+      </c>
+      <c r="C25" t="str">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>106</v>
+      </c>
+      <c r="E25">
+        <v>57</v>
+      </c>
+      <c r="F25">
+        <v>96</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:G32" si="0">MOD(D25-E25-F25,26)+F25</f>
+        <v>101</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" ref="H25:H32" si="1">CHAR(G25)</f>
+        <v>e</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <v>c</v>
+      </c>
+      <c r="C26" t="str">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>99</v>
+      </c>
+      <c r="E26">
+        <v>57</v>
+      </c>
+      <c r="F26">
+        <v>96</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <v>c</v>
+      </c>
+      <c r="C27" t="str">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>99</v>
+      </c>
+      <c r="E27">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <v>96</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <v>m</v>
+      </c>
+      <c r="C28" t="str">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>109</v>
+      </c>
+      <c r="E28">
+        <v>49</v>
+      </c>
+      <c r="F28">
+        <v>96</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>p</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <v>g</v>
+      </c>
+      <c r="C29" t="str">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>103</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <v>96</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>i</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <v>z</v>
+      </c>
+      <c r="C30" t="str">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>122</v>
+      </c>
+      <c r="E30">
+        <v>51</v>
+      </c>
+      <c r="F30">
+        <v>96</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <v>p</v>
+      </c>
+      <c r="C31" t="str">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>112</v>
+      </c>
+      <c r="E31">
+        <v>49</v>
+      </c>
+      <c r="F31">
+        <v>96</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>s</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <v>o</v>
+      </c>
+      <c r="C32" t="str">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>111</v>
+      </c>
+      <c r="E32">
+        <v>49</v>
+      </c>
+      <c r="F32">
+        <v>96</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>r</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Was able to breakdown Alt. Now figure out the logic
</commit_message>
<xml_diff>
--- a/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
+++ b/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80214398-0B9F-4EA8-A62E-C63E0D8FD910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF4E8C4-FA25-47B2-A06E-13CE22CC9CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1667,39 +1667,39 @@
             _xlpm.s, _xlfn.SEQUENCE(LEN(_xlpm.a)),
             _xlpm.c, CODE(MID(_xlpm.a, _xlpm.s, 1)),
             _xlpm.f, FLOOR(_xlpm.c, 32),
-            _xlfn.CONCAT(CHAR(MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26) + _xlpm.f),_xlpm.f,MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26))
+            _xlfn.CONCAT(CHAR(MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26) + _xlpm.f),"|",_xlpm.f,"|",MOD(_xlpm.c - MID(REPT(_xlpm.k, 9), _xlpm.s, 1) - _xlpm.f, 26))
         )
     )
 )</f>
-        <v>enemy969696969651451325</v>
+        <v>enemy|9696969696|51451325</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <v>battlewon969696969696969696212020125231514</v>
+        <v>battlewon|969696969696969696|212020125231514</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
-        <v>bringelephants9696969696969696969696969696218914751251681142019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>bringelephants|9696969696969696969696969696|218914751251681142019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
-        <v>moveforwardarchers9696969696969696969696969696969696961315225615182311841183851819</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>moveforwardarchers|969696969696969696969696969696969696|1315225615182311841183851819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
-        <v>horsesandcannons9696969696969696969696969696969681518195191144311414151419</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>horsesandcannons|96969696969696969696969696969696|81518195191144311414151419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
-        <v>hailthekingandqueen96969696969696969696969696969696969696819122085119147114417215514</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>hailthekingandqueen|96969696969696969696969696969696969696|819122085119147114417215514</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>19</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" t="str" cm="1">
         <f t="array" ref="B24:B32">MID(A3,_xlfn.SEQUENCE(LEN(A3)),1)</f>
         <v>c</v>
@@ -1732,15 +1732,19 @@
         <v>96</v>
       </c>
       <c r="G24">
-        <f>MOD(D24-E24-F24,26)+F24</f>
-        <v>102</v>
-      </c>
-      <c r="H24" t="str">
-        <f>CHAR(G24)</f>
-        <v>f</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <f>MOD(D24-C24-F24,26)</f>
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <f>F24+G24</f>
+        <v>98</v>
+      </c>
+      <c r="I24" t="str">
+        <f>CHAR(H24)</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <v>j</v>
       </c>
@@ -1757,15 +1761,19 @@
         <v>96</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25:G32" si="0">MOD(D25-E25-F25,26)+F25</f>
-        <v>101</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" ref="H25:H32" si="1">CHAR(G25)</f>
-        <v>e</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <f t="shared" ref="G25:G32" si="0">MOD(D25-C25-F25,26)</f>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H32" si="1">F25+G25</f>
+        <v>97</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" ref="I25:I32" si="2">CHAR(H25)</f>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <v>c</v>
       </c>
@@ -1783,14 +1791,18 @@
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="H26" t="str">
+        <v>20</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="1"/>
-        <v>x</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>t</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <v>c</v>
       </c>
@@ -1808,14 +1820,18 @@
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="H27" t="str">
+        <v>20</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="1"/>
-        <v>x</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>t</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <v>m</v>
       </c>
@@ -1833,14 +1849,18 @@
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-      <c r="H28" t="str">
+        <v>12</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="1"/>
-        <v>p</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>l</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
         <v>g</v>
       </c>
@@ -1858,14 +1878,18 @@
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="H29" t="str">
+        <v>5</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="1"/>
-        <v>i</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>e</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
         <v>z</v>
       </c>
@@ -1883,14 +1907,18 @@
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="H30" t="str">
+        <v>23</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="1"/>
-        <v>a</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>w</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <v>p</v>
       </c>
@@ -1908,14 +1936,18 @@
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-      <c r="H31" t="str">
+        <v>15</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>o</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <v>o</v>
       </c>
@@ -1933,11 +1965,15 @@
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-      <c r="H32" t="str">
+        <v>14</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="1"/>
-        <v>r</v>
+        <v>110</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="2"/>
+        <v>n</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I still am working on the use of the Floor function
</commit_message>
<xml_diff>
--- a/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
+++ b/Excel_Challenge_492 - Date Shift Cipher Decrypter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE3F96-A9F4-4D79-AE43-3496AFDF5ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7325C988-5C13-4D24-8891-8967F7D80BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1563,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6984DD-D8E9-4573-95DB-78BA80017482}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,14 +1989,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12A80B4-2B77-4EA2-A478-E0B7D909BD15}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>

</xml_diff>